<commit_message>
Update input sample file to exactly match the export format from the Operations Monitor.
</commit_message>
<xml_diff>
--- a/input/input-sample.xlsx
+++ b/input/input-sample.xlsx
@@ -21,13 +21,13 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t>TaskPath</t>
+    <t>Reload of Extract Script - Sales &gt;&gt; Reload of Fact - Sales &gt;&gt; Reload of Data Model - Sales and Marketing &gt;&gt; Reload of Dashboard - Sales and Marketing</t>
   </si>
   <si>
-    <t>TaskDepth</t>
+    <t>Task Path</t>
   </si>
   <si>
-    <t>Reload of Extract Script - Sales &gt;&gt; Reload of Fact - Sales &gt;&gt; Reload of Data Model - Sales and Marketing &gt;&gt; Reload of Dashboard - Sales and Marketing</t>
+    <t>Depth</t>
   </si>
 </sst>
 </file>
@@ -63,10 +63,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -375,28 +378,28 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="166.5703125" customWidth="1"/>
+    <col min="1" max="1" width="134.140625" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2">
+      <c r="B2" s="2">
         <v>4</v>
       </c>
     </row>

</xml_diff>